<commit_message>
early version under construction
</commit_message>
<xml_diff>
--- a/ccr_data(0.2).xlsx
+++ b/ccr_data(0.2).xlsx
@@ -806,7 +806,7 @@
   <dimension ref="B1:G50"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -871,7 +871,9 @@
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="3"/>
-      <c r="C7" s="16"/>
+      <c r="C7" s="16" t="s">
+        <v>49</v>
+      </c>
       <c r="D7" s="18" t="s">
         <v>37</v>
       </c>
@@ -887,9 +889,7 @@
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="3"/>
-      <c r="C8" s="16" t="s">
-        <v>49</v>
-      </c>
+      <c r="C8" s="16"/>
       <c r="D8" s="18" t="s">
         <v>37</v>
       </c>

</xml_diff>